<commit_message>
Enhance the CustomProcessUpload sample with import BPMN use case
</commit_message>
<xml_diff>
--- a/applications/CustomProcessUpload/input/Sample Content Public.xlsx
+++ b/applications/CustomProcessUpload/input/Sample Content Public.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d033027/Documents/GitHub/cloud-alm-api-examples/applications/CustomProcessUpload/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I542511\Desktop\my-projects\cloud-alm-api-examples\applications\CustomProcessUpload\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB3EBF04-D888-7A4B-82DA-79D5A189C360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E0FC97-2286-46C5-BD4F-CA2C39234373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36120" yWindow="2820" windowWidth="30660" windowHeight="18840" xr2:uid="{B8E33C24-D37B-4E02-B9ED-3DBD4120E97F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B8E33C24-D37B-4E02-B9ED-3DBD4120E97F}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>../input/diagrams/Idea-to-Market/SPF Handover new Material.svg</t>
-  </si>
-  <si>
-    <t>../input/diagrams/Idea-to-Market/SPF Handover to Manufacturing.svg</t>
   </si>
   <si>
     <t>../input/diagrams/Idea-to-Market/SPF Create Detailed Design.svg</t>
@@ -193,19 +190,25 @@
     <t>../input/diagrams/Lead-to-Cash/SVF Lead to Cash for Hybrid Deployment.svg</t>
   </si>
   <si>
+    <t>BPMN</t>
+  </si>
+  <si>
+    <t>../input/diagrams/Idea-to-Market/SPF Handover to Manufacturing.bpmn2</t>
+  </si>
+  <si>
+    <t>&lt;your company&gt;</t>
+  </si>
+  <si>
+    <t>&lt;your tenant url&gt;</t>
+  </si>
+  <si>
+    <t>&lt;your auth url&gt;</t>
+  </si>
+  <si>
+    <t>&lt;your client id&gt;</t>
+  </si>
+  <si>
     <t>&lt;your secret&gt;</t>
-  </si>
-  <si>
-    <t>&lt;your client id&gt;</t>
-  </si>
-  <si>
-    <t>&lt;your auth url&gt;</t>
-  </si>
-  <si>
-    <t>&lt;your tenant url&gt;</t>
-  </si>
-  <si>
-    <t>&lt;your company&gt;</t>
   </si>
 </sst>
 </file>
@@ -378,11 +381,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A65DFB0B-E920-254A-A665-92B1CC244F1F}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6" xr:uid="{A65DFB0B-E920-254A-A665-92B1CC244F1F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1237BF58-0409-43B9-9CB7-510D76CDA13E}" name="Table17" displayName="Table17" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{1237BF58-0409-43B9-9CB7-510D76CDA13E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D3315670-70D2-5D41-8CDF-4C2DDB866BAE}" name="Property"/>
-    <tableColumn id="2" xr3:uid="{A680009C-F5ED-8442-96FA-7D477C03970C}" name="Value"/>
+    <tableColumn id="1" xr3:uid="{4345AA8E-A4E6-4BAA-A434-4F5ABA72AC25}" name="Property"/>
+    <tableColumn id="2" xr3:uid="{758C1D5A-5786-4269-9B46-191C45ED7404}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -403,13 +406,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F25254C3-E260-BD48-AB21-1BDEADC46A56}" name="Table4" displayName="Table4" ref="A1:D7" totalsRowShown="0">
-  <autoFilter ref="A1:D7" xr:uid="{F25254C3-E260-BD48-AB21-1BDEADC46A56}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F25254C3-E260-BD48-AB21-1BDEADC46A56}" name="Table4" displayName="Table4" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{F25254C3-E260-BD48-AB21-1BDEADC46A56}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{727000B3-AB0F-AD42-B572-216843286B0C}" name="Solution Process ID"/>
     <tableColumn id="2" xr3:uid="{6286BEE7-DD99-AF46-AFF1-C3690AB7720A}" name="Type"/>
     <tableColumn id="3" xr3:uid="{8A53DB8D-001F-E14E-82EC-8B3D59F3AD24}" name="Diagram Name"/>
     <tableColumn id="4" xr3:uid="{ABF19370-D096-0C49-9DFA-29AB97DF6EFC}" name="SVG"/>
+    <tableColumn id="5" xr3:uid="{49630EAD-5DAC-4BE6-8156-37A8FFBBAD38}" name="BPMN"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -728,17 +732,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272BA4B8-DF98-5E44-87D2-313208B6F684}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="33.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -746,54 +746,55 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://calm-dev-eu10-004-relcallstablefeatures-1stabledata.dev.eu10.alm.cloud.sap" xr:uid="{B79E5644-9567-C94A-B077-B064DAA72616}"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://calm-dev-eu10-004-relcallstablefeatures-1stabledata.authentication.eu10.hana.ondemand.com" xr:uid="{DBC03AB7-9DB7-B741-BDFA-050E139A9492}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://calm-dev-eu10-004-relcallstablefeatures-1stabledata.dev.eu10.alm.cloud.sap" xr:uid="{42429872-3169-4DEE-B8DC-895D99EE8231}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://calm-dev-eu10-004-relcallstablefeatures-1stabledata.authentication.eu10.hana.ondemand.com" xr:uid="{DC01983F-8746-4F15-A639-B0142A43134D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -804,20 +805,20 @@
   <dimension ref="A1:E259"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="2"/>
+    <col min="1" max="1" width="11.44140625" style="2"/>
     <col min="2" max="2" width="43" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="2"/>
+    <col min="3" max="3" width="32.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="2"/>
     <col min="5" max="5" width="59.6640625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="2"/>
+    <col min="6" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -834,7 +835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -851,789 +852,789 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E56" s="3"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E57" s="3"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E58" s="3"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E59" s="3"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E60" s="3"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E62" s="3"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E65" s="3"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E66" s="3"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67" s="3"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E68" s="3"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E69" s="3"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E70" s="3"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E71" s="3"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E72" s="3"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E73" s="3"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E74" s="3"/>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E75" s="3"/>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E76" s="3"/>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E77" s="3"/>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E78" s="3"/>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E79" s="3"/>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E80" s="3"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E81" s="3"/>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E82" s="3"/>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E83" s="3"/>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E84" s="3"/>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E85" s="3"/>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E86" s="3"/>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E87" s="3"/>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E88" s="3"/>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E89" s="3"/>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E90" s="3"/>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E91" s="3"/>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E92" s="3"/>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E93" s="3"/>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E94" s="3"/>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E95" s="3"/>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E96" s="3"/>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E97" s="3"/>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E98" s="3"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E99" s="3"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E100" s="3"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E101" s="3"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E102" s="3"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E103" s="3"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E104" s="3"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E105" s="3"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E106" s="3"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E107" s="3"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E108" s="3"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E109" s="3"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E110" s="3"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E111" s="3"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E112" s="3"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E113" s="3"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E114" s="3"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E115" s="3"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E116" s="3"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E117" s="3"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E118" s="3"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E119" s="3"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E120" s="3"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E121" s="3"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E122" s="3"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E123" s="3"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E124" s="3"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E125" s="3"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E126" s="3"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E127" s="3"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E128" s="3"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E129" s="3"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E130" s="3"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E131" s="3"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E132" s="3"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E133" s="3"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E134" s="3"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E135" s="3"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E136" s="3"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E137" s="3"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E138" s="3"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E139" s="3"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E140" s="3"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E141" s="3"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E142" s="3"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E143" s="3"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E144" s="3"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E145" s="3"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E146" s="3"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E147" s="3"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E148" s="3"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E149" s="3"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E150" s="3"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E151" s="3"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E152" s="3"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E153" s="3"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E154" s="3"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E155" s="3"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E156" s="3"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E157" s="3"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E158" s="3"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E159" s="3"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E160" s="3"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E161" s="3"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E162" s="3"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E163" s="3"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E164" s="3"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E165" s="3"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E166" s="3"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E167" s="3"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E168" s="3"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E169" s="3"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E170" s="3"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E171" s="3"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E172" s="3"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E173" s="3"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E174" s="3"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E175" s="3"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E176" s="3"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E177" s="3"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E178" s="3"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E179" s="3"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E180" s="3"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E181" s="3"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E182" s="3"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E183" s="3"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E184" s="3"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E185" s="3"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E186" s="3"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E187" s="3"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E188" s="3"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E189" s="3"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E190" s="3"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E191" s="3"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E192" s="3"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E193" s="3"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E194" s="3"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E195" s="3"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E196" s="3"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E197" s="3"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E198" s="3"/>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E199" s="3"/>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E200" s="3"/>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E201" s="3"/>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E202" s="3"/>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E203" s="3"/>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E204" s="3"/>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E205" s="3"/>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E206" s="3"/>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E207" s="3"/>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E208" s="3"/>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="209" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E209" s="3"/>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="210" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E210" s="3"/>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="211" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E211" s="3"/>
     </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="212" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E212" s="3"/>
     </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="213" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E213" s="3"/>
     </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="214" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E214" s="3"/>
     </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="215" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E215" s="3"/>
     </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="216" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E216" s="3"/>
     </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="217" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E217" s="3"/>
     </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="218" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E218" s="3"/>
     </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="219" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E219" s="3"/>
     </row>
-    <row r="220" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="220" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E220" s="3"/>
     </row>
-    <row r="221" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="221" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E221" s="3"/>
     </row>
-    <row r="222" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="222" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E222" s="3"/>
     </row>
-    <row r="223" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="223" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E223" s="3"/>
     </row>
-    <row r="224" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="224" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E224" s="3"/>
     </row>
-    <row r="225" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="225" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E225" s="3"/>
     </row>
-    <row r="226" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="226" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E226" s="3"/>
     </row>
-    <row r="227" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="227" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E227" s="3"/>
     </row>
-    <row r="228" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="228" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E228" s="3"/>
     </row>
-    <row r="229" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="229" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E229" s="3"/>
     </row>
-    <row r="230" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="230" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E230" s="3"/>
     </row>
-    <row r="231" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E231" s="3"/>
     </row>
-    <row r="232" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="232" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E232" s="3"/>
     </row>
-    <row r="233" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="233" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E233" s="3"/>
     </row>
-    <row r="234" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="234" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E234" s="3"/>
     </row>
-    <row r="235" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="235" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E235" s="3"/>
     </row>
-    <row r="236" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="236" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E236" s="3"/>
     </row>
-    <row r="237" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="237" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E237" s="3"/>
     </row>
-    <row r="238" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="238" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E238" s="3"/>
     </row>
-    <row r="239" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="239" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E239" s="3"/>
     </row>
-    <row r="240" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="240" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E240" s="3"/>
     </row>
-    <row r="241" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="241" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E241" s="3"/>
     </row>
-    <row r="242" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="242" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E242" s="3"/>
     </row>
-    <row r="243" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="243" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E243" s="3"/>
     </row>
-    <row r="244" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="244" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E244" s="3"/>
     </row>
-    <row r="245" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="245" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E245" s="3"/>
     </row>
-    <row r="246" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="246" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E246" s="3"/>
     </row>
-    <row r="247" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="247" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E247" s="3"/>
     </row>
-    <row r="248" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="248" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E248" s="3"/>
     </row>
-    <row r="249" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="249" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E249" s="3"/>
     </row>
-    <row r="250" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="250" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E250" s="3"/>
     </row>
-    <row r="251" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="251" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E251" s="3"/>
     </row>
-    <row r="252" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="252" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E252" s="3"/>
     </row>
-    <row r="253" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="253" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E253" s="3"/>
     </row>
-    <row r="254" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="254" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E254" s="3"/>
     </row>
-    <row r="255" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="255" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E255" s="3"/>
     </row>
-    <row r="256" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="256" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E256" s="3"/>
     </row>
-    <row r="257" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="257" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E257" s="3"/>
     </row>
-    <row r="258" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="258" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E258" s="3"/>
     </row>
-    <row r="259" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="259" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E259" s="3"/>
     </row>
   </sheetData>
@@ -1649,21 +1650,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C451A2-0A09-A740-B673-B25D0AEDB855}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
     <col min="3" max="3" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.77734375" customWidth="1"/>
+    <col min="5" max="5" width="68.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1676,8 +1678,11 @@
       <c r="D1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1691,7 +1696,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1699,13 +1704,13 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1713,13 +1718,13 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1727,13 +1732,13 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1741,31 +1746,32 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1779,16 +1785,16 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="104.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1805,7 +1811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1822,7 +1828,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1839,7 +1845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1856,9 +1862,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -1870,7 +1876,7 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1890,14 +1896,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d0ed3ca2-9f65-48f7-b860-393f60d04052" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9483849f-e75d-423c-a8ca-6edae6e70315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2118,27 +2122,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d0ed3ca2-9f65-48f7-b860-393f60d04052" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9483849f-e75d-423c-a8ca-6edae6e70315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{102828BE-4020-41D9-A855-B87294169A3B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3537408-77DA-490F-A9A5-F913C491DAD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d0ed3ca2-9f65-48f7-b860-393f60d04052"/>
-    <ds:schemaRef ds:uri="9483849f-e75d-423c-a8ca-6edae6e70315"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2163,9 +2160,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3537408-77DA-490F-A9A5-F913C491DAD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{102828BE-4020-41D9-A855-B87294169A3B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d0ed3ca2-9f65-48f7-b860-393f60d04052"/>
+    <ds:schemaRef ds:uri="9483849f-e75d-423c-a8ca-6edae6e70315"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Enhance the CustomProcessUpload sample with import BPMN use case (#27)
Co-authored-by: I542511 <m.hidri@sap.com>
</commit_message>
<xml_diff>
--- a/applications/CustomProcessUpload/input/Sample Content Public.xlsx
+++ b/applications/CustomProcessUpload/input/Sample Content Public.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d033027/Documents/GitHub/cloud-alm-api-examples/applications/CustomProcessUpload/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I542511\Desktop\my-projects\cloud-alm-api-examples\applications\CustomProcessUpload\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB3EBF04-D888-7A4B-82DA-79D5A189C360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E0FC97-2286-46C5-BD4F-CA2C39234373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36120" yWindow="2820" windowWidth="30660" windowHeight="18840" xr2:uid="{B8E33C24-D37B-4E02-B9ED-3DBD4120E97F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B8E33C24-D37B-4E02-B9ED-3DBD4120E97F}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>../input/diagrams/Idea-to-Market/SPF Handover new Material.svg</t>
-  </si>
-  <si>
-    <t>../input/diagrams/Idea-to-Market/SPF Handover to Manufacturing.svg</t>
   </si>
   <si>
     <t>../input/diagrams/Idea-to-Market/SPF Create Detailed Design.svg</t>
@@ -193,19 +190,25 @@
     <t>../input/diagrams/Lead-to-Cash/SVF Lead to Cash for Hybrid Deployment.svg</t>
   </si>
   <si>
+    <t>BPMN</t>
+  </si>
+  <si>
+    <t>../input/diagrams/Idea-to-Market/SPF Handover to Manufacturing.bpmn2</t>
+  </si>
+  <si>
+    <t>&lt;your company&gt;</t>
+  </si>
+  <si>
+    <t>&lt;your tenant url&gt;</t>
+  </si>
+  <si>
+    <t>&lt;your auth url&gt;</t>
+  </si>
+  <si>
+    <t>&lt;your client id&gt;</t>
+  </si>
+  <si>
     <t>&lt;your secret&gt;</t>
-  </si>
-  <si>
-    <t>&lt;your client id&gt;</t>
-  </si>
-  <si>
-    <t>&lt;your auth url&gt;</t>
-  </si>
-  <si>
-    <t>&lt;your tenant url&gt;</t>
-  </si>
-  <si>
-    <t>&lt;your company&gt;</t>
   </si>
 </sst>
 </file>
@@ -378,11 +381,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A65DFB0B-E920-254A-A665-92B1CC244F1F}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6" xr:uid="{A65DFB0B-E920-254A-A665-92B1CC244F1F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1237BF58-0409-43B9-9CB7-510D76CDA13E}" name="Table17" displayName="Table17" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{1237BF58-0409-43B9-9CB7-510D76CDA13E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D3315670-70D2-5D41-8CDF-4C2DDB866BAE}" name="Property"/>
-    <tableColumn id="2" xr3:uid="{A680009C-F5ED-8442-96FA-7D477C03970C}" name="Value"/>
+    <tableColumn id="1" xr3:uid="{4345AA8E-A4E6-4BAA-A434-4F5ABA72AC25}" name="Property"/>
+    <tableColumn id="2" xr3:uid="{758C1D5A-5786-4269-9B46-191C45ED7404}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -403,13 +406,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F25254C3-E260-BD48-AB21-1BDEADC46A56}" name="Table4" displayName="Table4" ref="A1:D7" totalsRowShown="0">
-  <autoFilter ref="A1:D7" xr:uid="{F25254C3-E260-BD48-AB21-1BDEADC46A56}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F25254C3-E260-BD48-AB21-1BDEADC46A56}" name="Table4" displayName="Table4" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{F25254C3-E260-BD48-AB21-1BDEADC46A56}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{727000B3-AB0F-AD42-B572-216843286B0C}" name="Solution Process ID"/>
     <tableColumn id="2" xr3:uid="{6286BEE7-DD99-AF46-AFF1-C3690AB7720A}" name="Type"/>
     <tableColumn id="3" xr3:uid="{8A53DB8D-001F-E14E-82EC-8B3D59F3AD24}" name="Diagram Name"/>
     <tableColumn id="4" xr3:uid="{ABF19370-D096-0C49-9DFA-29AB97DF6EFC}" name="SVG"/>
+    <tableColumn id="5" xr3:uid="{49630EAD-5DAC-4BE6-8156-37A8FFBBAD38}" name="BPMN"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -728,17 +732,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272BA4B8-DF98-5E44-87D2-313208B6F684}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="33.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -746,54 +746,55 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://calm-dev-eu10-004-relcallstablefeatures-1stabledata.dev.eu10.alm.cloud.sap" xr:uid="{B79E5644-9567-C94A-B077-B064DAA72616}"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://calm-dev-eu10-004-relcallstablefeatures-1stabledata.authentication.eu10.hana.ondemand.com" xr:uid="{DBC03AB7-9DB7-B741-BDFA-050E139A9492}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://calm-dev-eu10-004-relcallstablefeatures-1stabledata.dev.eu10.alm.cloud.sap" xr:uid="{42429872-3169-4DEE-B8DC-895D99EE8231}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://calm-dev-eu10-004-relcallstablefeatures-1stabledata.authentication.eu10.hana.ondemand.com" xr:uid="{DC01983F-8746-4F15-A639-B0142A43134D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -804,20 +805,20 @@
   <dimension ref="A1:E259"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="2"/>
+    <col min="1" max="1" width="11.44140625" style="2"/>
     <col min="2" max="2" width="43" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="2"/>
+    <col min="3" max="3" width="32.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="2"/>
     <col min="5" max="5" width="59.6640625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="2"/>
+    <col min="6" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -834,7 +835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -851,789 +852,789 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E56" s="3"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E57" s="3"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E58" s="3"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E59" s="3"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E60" s="3"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E62" s="3"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E65" s="3"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E66" s="3"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67" s="3"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E68" s="3"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E69" s="3"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E70" s="3"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E71" s="3"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E72" s="3"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E73" s="3"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E74" s="3"/>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E75" s="3"/>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E76" s="3"/>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E77" s="3"/>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E78" s="3"/>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E79" s="3"/>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E80" s="3"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E81" s="3"/>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E82" s="3"/>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E83" s="3"/>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E84" s="3"/>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E85" s="3"/>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E86" s="3"/>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E87" s="3"/>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E88" s="3"/>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E89" s="3"/>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E90" s="3"/>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E91" s="3"/>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E92" s="3"/>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E93" s="3"/>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E94" s="3"/>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E95" s="3"/>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E96" s="3"/>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E97" s="3"/>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E98" s="3"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E99" s="3"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E100" s="3"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E101" s="3"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E102" s="3"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E103" s="3"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E104" s="3"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E105" s="3"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E106" s="3"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E107" s="3"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E108" s="3"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E109" s="3"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E110" s="3"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E111" s="3"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E112" s="3"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E113" s="3"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E114" s="3"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E115" s="3"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E116" s="3"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E117" s="3"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E118" s="3"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E119" s="3"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E120" s="3"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E121" s="3"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E122" s="3"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E123" s="3"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E124" s="3"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E125" s="3"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E126" s="3"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E127" s="3"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E128" s="3"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E129" s="3"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E130" s="3"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E131" s="3"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E132" s="3"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E133" s="3"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E134" s="3"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E135" s="3"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E136" s="3"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E137" s="3"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E138" s="3"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E139" s="3"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E140" s="3"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E141" s="3"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E142" s="3"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E143" s="3"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E144" s="3"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E145" s="3"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E146" s="3"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E147" s="3"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E148" s="3"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E149" s="3"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E150" s="3"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E151" s="3"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E152" s="3"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E153" s="3"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E154" s="3"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E155" s="3"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E156" s="3"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E157" s="3"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E158" s="3"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E159" s="3"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E160" s="3"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E161" s="3"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E162" s="3"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E163" s="3"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E164" s="3"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E165" s="3"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E166" s="3"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E167" s="3"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E168" s="3"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E169" s="3"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E170" s="3"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E171" s="3"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E172" s="3"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E173" s="3"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E174" s="3"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E175" s="3"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E176" s="3"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E177" s="3"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E178" s="3"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E179" s="3"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E180" s="3"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E181" s="3"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E182" s="3"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E183" s="3"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E184" s="3"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E185" s="3"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E186" s="3"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E187" s="3"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E188" s="3"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E189" s="3"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E190" s="3"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E191" s="3"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E192" s="3"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E193" s="3"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E194" s="3"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E195" s="3"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E196" s="3"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E197" s="3"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E198" s="3"/>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E199" s="3"/>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E200" s="3"/>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E201" s="3"/>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E202" s="3"/>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E203" s="3"/>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E204" s="3"/>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E205" s="3"/>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E206" s="3"/>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E207" s="3"/>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E208" s="3"/>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="209" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E209" s="3"/>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="210" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E210" s="3"/>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="211" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E211" s="3"/>
     </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="212" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E212" s="3"/>
     </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="213" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E213" s="3"/>
     </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="214" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E214" s="3"/>
     </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="215" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E215" s="3"/>
     </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="216" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E216" s="3"/>
     </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="217" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E217" s="3"/>
     </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="218" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E218" s="3"/>
     </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="219" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E219" s="3"/>
     </row>
-    <row r="220" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="220" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E220" s="3"/>
     </row>
-    <row r="221" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="221" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E221" s="3"/>
     </row>
-    <row r="222" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="222" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E222" s="3"/>
     </row>
-    <row r="223" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="223" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E223" s="3"/>
     </row>
-    <row r="224" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="224" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E224" s="3"/>
     </row>
-    <row r="225" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="225" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E225" s="3"/>
     </row>
-    <row r="226" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="226" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E226" s="3"/>
     </row>
-    <row r="227" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="227" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E227" s="3"/>
     </row>
-    <row r="228" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="228" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E228" s="3"/>
     </row>
-    <row r="229" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="229" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E229" s="3"/>
     </row>
-    <row r="230" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="230" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E230" s="3"/>
     </row>
-    <row r="231" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E231" s="3"/>
     </row>
-    <row r="232" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="232" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E232" s="3"/>
     </row>
-    <row r="233" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="233" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E233" s="3"/>
     </row>
-    <row r="234" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="234" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E234" s="3"/>
     </row>
-    <row r="235" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="235" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E235" s="3"/>
     </row>
-    <row r="236" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="236" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E236" s="3"/>
     </row>
-    <row r="237" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="237" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E237" s="3"/>
     </row>
-    <row r="238" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="238" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E238" s="3"/>
     </row>
-    <row r="239" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="239" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E239" s="3"/>
     </row>
-    <row r="240" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="240" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E240" s="3"/>
     </row>
-    <row r="241" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="241" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E241" s="3"/>
     </row>
-    <row r="242" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="242" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E242" s="3"/>
     </row>
-    <row r="243" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="243" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E243" s="3"/>
     </row>
-    <row r="244" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="244" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E244" s="3"/>
     </row>
-    <row r="245" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="245" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E245" s="3"/>
     </row>
-    <row r="246" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="246" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E246" s="3"/>
     </row>
-    <row r="247" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="247" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E247" s="3"/>
     </row>
-    <row r="248" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="248" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E248" s="3"/>
     </row>
-    <row r="249" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="249" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E249" s="3"/>
     </row>
-    <row r="250" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="250" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E250" s="3"/>
     </row>
-    <row r="251" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="251" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E251" s="3"/>
     </row>
-    <row r="252" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="252" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E252" s="3"/>
     </row>
-    <row r="253" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="253" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E253" s="3"/>
     </row>
-    <row r="254" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="254" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E254" s="3"/>
     </row>
-    <row r="255" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="255" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E255" s="3"/>
     </row>
-    <row r="256" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="256" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E256" s="3"/>
     </row>
-    <row r="257" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="257" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E257" s="3"/>
     </row>
-    <row r="258" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="258" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E258" s="3"/>
     </row>
-    <row r="259" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="259" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E259" s="3"/>
     </row>
   </sheetData>
@@ -1649,21 +1650,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C451A2-0A09-A740-B673-B25D0AEDB855}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
     <col min="3" max="3" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.77734375" customWidth="1"/>
+    <col min="5" max="5" width="68.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1676,8 +1678,11 @@
       <c r="D1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1691,7 +1696,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1699,13 +1704,13 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1713,13 +1718,13 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1727,13 +1732,13 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1741,31 +1746,32 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1779,16 +1785,16 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="104.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1805,7 +1811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1822,7 +1828,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1839,7 +1845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1856,9 +1862,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -1870,7 +1876,7 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1890,14 +1896,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d0ed3ca2-9f65-48f7-b860-393f60d04052" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9483849f-e75d-423c-a8ca-6edae6e70315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2118,27 +2122,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d0ed3ca2-9f65-48f7-b860-393f60d04052" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9483849f-e75d-423c-a8ca-6edae6e70315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{102828BE-4020-41D9-A855-B87294169A3B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3537408-77DA-490F-A9A5-F913C491DAD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d0ed3ca2-9f65-48f7-b860-393f60d04052"/>
-    <ds:schemaRef ds:uri="9483849f-e75d-423c-a8ca-6edae6e70315"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2163,9 +2160,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3537408-77DA-490F-A9A5-F913C491DAD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{102828BE-4020-41D9-A855-B87294169A3B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d0ed3ca2-9f65-48f7-b860-393f60d04052"/>
+    <ds:schemaRef ds:uri="9483849f-e75d-423c-a8ca-6edae6e70315"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>